<commit_message>
add some SMS examples.
</commit_message>
<xml_diff>
--- a/app/tables/send_sms/forms/send_sms/send_sms.xlsx
+++ b/app/tables/send_sms/forms/send_sms/send_sms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>type</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>Enter the subject's name.</t>
+  </si>
+  <si>
+    <t>odk_sms</t>
+  </si>
+  <si>
+    <t>This will send an sms via the sms bridge.</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>Enter the phone number to which to send the text.</t>
+  </si>
+  <si>
+    <t>odk_sms_automatic</t>
+  </si>
+  <si>
+    <t>This will send an sms without requiring confirmation.</t>
   </si>
 </sst>
 </file>
@@ -429,16 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="102.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
@@ -472,18 +490,51 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="12">
       <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -500,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -526,8 +577,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1"/>
-    <row r="4" spans="1:2" ht="15" customHeight="1"/>
+    <row r="3" spans="1:2" ht="15" customHeight="1">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>